<commit_message>
Additions to ab06 and ab16 translation rules; updates to cas specs.
</commit_message>
<xml_diff>
--- a/docs/specifications/errors/cas_errors.xlsx
+++ b/docs/specifications/errors/cas_errors.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20341"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20342"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA2333F-34F0-4B7A-BF73-F2B6F3256ADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA7B49-7915-42E3-A248-EB887CE27D6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30110" yWindow="540" windowWidth="19070" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30110" yWindow="540" windowWidth="19070" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Short v3" sheetId="4" r:id="rId1"/>
-    <sheet name="Long v3" sheetId="3" r:id="rId2"/>
-    <sheet name="Specific codes" sheetId="5" r:id="rId3"/>
-    <sheet name="version 2" sheetId="2" r:id="rId4"/>
-    <sheet name="version 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Readme" sheetId="6" r:id="rId1"/>
+    <sheet name="cas_errors_general" sheetId="4" r:id="rId2"/>
+    <sheet name="cas_errors_specific" sheetId="5" r:id="rId3"/>
+    <sheet name="version 3" sheetId="3" r:id="rId4"/>
+    <sheet name="version 2" sheetId="2" r:id="rId5"/>
+    <sheet name="version 1" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="151">
   <si>
     <t>CAS04_code</t>
   </si>
@@ -502,13 +503,46 @@
   </si>
   <si>
     <t>Error_type</t>
+  </si>
+  <si>
+    <t>Worksheet</t>
+  </si>
+  <si>
+    <t>cas_errors_general</t>
+  </si>
+  <si>
+    <t>cas_errors_specific</t>
+  </si>
+  <si>
+    <t>version 3</t>
+  </si>
+  <si>
+    <t>version 2</t>
+  </si>
+  <si>
+    <t>version 1</t>
+  </si>
+  <si>
+    <t>General error codes; extracted from version 3 worksheet; save to csv format for github</t>
+  </si>
+  <si>
+    <t>Attribute-specific error codes; extracted from version 3 worksheet; save to csv format for github</t>
+  </si>
+  <si>
+    <t>Latest working copy of error codes (March 2019)</t>
+  </si>
+  <si>
+    <t>Version 2 of error codes (February 2019)</t>
+  </si>
+  <si>
+    <t>Version 1 of error codes (January 2019)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,6 +578,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -559,7 +601,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -576,11 +618,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -601,9 +654,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -647,15 +697,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,280 +1094,346 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA204F2A-D47C-4AF9-9747-36349398920E}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA55EC8-7307-4427-942B-5F374DD8C01A}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.90625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.54296875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <v>-2222</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>-222222222</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <v>-2147483648</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>-2221</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>-222222221</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <v>2147483647</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>-8888</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>-888888888</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <v>-2147483647</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="B6" s="13" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>-8887</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>-888888887</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>-2147483645</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" ht="65" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>-9999</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>-999999999</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>-2147483644</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>-9998</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>-999999998</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <v>-2147483643</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>-9997</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>-999999997</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>-2147483642</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>-9996</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>-999999996</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>-2147483641</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="18" t="s">
+    <row r="11" spans="1:8" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20"/>
+      <c r="B11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="19">
         <v>-9995</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="19">
         <v>-999999995</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="19">
         <v>-2147483640</v>
       </c>
     </row>
@@ -1303,719 +1444,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C433B836-2E24-4019-9D1B-300F5E0548AB}">
-  <dimension ref="A1:L24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:K3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.54296875" style="1" customWidth="1"/>
-    <col min="2" max="12" width="20.54296875" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="8" customFormat="1" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="8" customFormat="1" ht="78.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>-8888</v>
-      </c>
-      <c r="F7" s="2">
-        <v>-1111</v>
-      </c>
-      <c r="H7" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="I7" s="2">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="2">
-        <v>-2222</v>
-      </c>
-      <c r="D9" s="2">
-        <v>-2221</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-8888</v>
-      </c>
-      <c r="G9" s="2">
-        <v>-8887</v>
-      </c>
-      <c r="H9" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="I9" s="2">
-        <v>-9998</v>
-      </c>
-      <c r="J9" s="2">
-        <v>-9997</v>
-      </c>
-      <c r="K9" s="2">
-        <v>-9996</v>
-      </c>
-      <c r="L9" s="2">
-        <v>-9995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-222222222</v>
-      </c>
-      <c r="D10" s="2">
-        <v>-222222221</v>
-      </c>
-      <c r="E10" s="2">
-        <v>-888888888</v>
-      </c>
-      <c r="G10" s="2">
-        <v>-888888887</v>
-      </c>
-      <c r="H10" s="2">
-        <v>-999999999</v>
-      </c>
-      <c r="I10" s="2">
-        <v>-999999998</v>
-      </c>
-      <c r="J10" s="2">
-        <v>-999999997</v>
-      </c>
-      <c r="K10" s="2">
-        <v>-999999996</v>
-      </c>
-      <c r="L10" s="2">
-        <v>-999999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="2">
-        <v>-32768</v>
-      </c>
-      <c r="D12" s="2">
-        <v>32767</v>
-      </c>
-      <c r="E12" s="2">
-        <v>-32767</v>
-      </c>
-      <c r="G12" s="2">
-        <v>-32765</v>
-      </c>
-      <c r="H12" s="2">
-        <v>-32764</v>
-      </c>
-      <c r="I12" s="2">
-        <v>-32763</v>
-      </c>
-      <c r="J12" s="2">
-        <v>-32762</v>
-      </c>
-      <c r="K12" s="2">
-        <v>-32761</v>
-      </c>
-      <c r="L12" s="2">
-        <v>-32760</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="2">
-        <v>-2147483648</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2147483647</v>
-      </c>
-      <c r="E13" s="2">
-        <v>-2147483647</v>
-      </c>
-      <c r="G13" s="2">
-        <v>-2147483645</v>
-      </c>
-      <c r="H13" s="2">
-        <v>-2147483644</v>
-      </c>
-      <c r="I13" s="2">
-        <v>-2147483643</v>
-      </c>
-      <c r="J13" s="2">
-        <v>-2147483642</v>
-      </c>
-      <c r="K13" s="2">
-        <v>-2147483641</v>
-      </c>
-      <c r="L13" s="2">
-        <v>-2147483640</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="2">
-        <v>-2147483648</v>
-      </c>
-      <c r="D14" s="2">
-        <v>2147483647</v>
-      </c>
-      <c r="E14" s="2">
-        <v>-2147483647</v>
-      </c>
-      <c r="G14" s="2">
-        <v>-2147483645</v>
-      </c>
-      <c r="H14" s="2">
-        <v>-2147483644</v>
-      </c>
-      <c r="I14" s="2">
-        <v>-2147483643</v>
-      </c>
-      <c r="J14" s="2">
-        <v>-2147483642</v>
-      </c>
-      <c r="K14" s="2">
-        <v>-2147483641</v>
-      </c>
-      <c r="L14" s="2">
-        <v>-2147483640</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="2">
-        <v>-2222</v>
-      </c>
-      <c r="D18" s="2">
-        <v>-2221</v>
-      </c>
-      <c r="E18" s="2">
-        <v>-8888</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G18" s="2">
-        <v>-8886</v>
-      </c>
-      <c r="H18" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J18" s="2">
-        <v>-9997</v>
-      </c>
-      <c r="K18" s="2">
-        <v>-9996</v>
-      </c>
-      <c r="L18" s="2">
-        <v>-9995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="2">
-        <v>-2222</v>
-      </c>
-      <c r="D19" s="2">
-        <v>-2221</v>
-      </c>
-      <c r="E19" s="2">
-        <v>-8888</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G19" s="2">
-        <v>-8886</v>
-      </c>
-      <c r="H19" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J19" s="2">
-        <v>-9997</v>
-      </c>
-      <c r="K19" s="2">
-        <v>-9996</v>
-      </c>
-      <c r="L19" s="2">
-        <v>-9995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="2">
-        <v>-8888</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G20" s="2">
-        <v>-8886</v>
-      </c>
-      <c r="H20" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="I20" s="2">
-        <v>-9998</v>
-      </c>
-      <c r="J20" s="2">
-        <v>-9997</v>
-      </c>
-      <c r="K20" s="2">
-        <v>-9996</v>
-      </c>
-      <c r="L20" s="2">
-        <v>-9995</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="2">
-        <v>-8888</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="2">
-        <v>-8886</v>
-      </c>
-      <c r="H21" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="I21" s="2">
-        <v>-9998</v>
-      </c>
-      <c r="J21" s="2">
-        <v>-9997</v>
-      </c>
-      <c r="K21" s="2">
-        <v>-9996</v>
-      </c>
-      <c r="L21" s="2">
-        <v>-9995</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" s="2">
-        <v>-8888</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G23" s="2">
-        <v>-8886</v>
-      </c>
-      <c r="H23" s="2">
-        <v>-9999</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J23" s="2">
-        <v>-9997</v>
-      </c>
-      <c r="K23" s="2">
-        <v>-9996</v>
-      </c>
-      <c r="L23" s="2">
-        <v>-9995</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C733A05B-0C07-42CA-BAFC-8B5F4B6FFF4B}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.36328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.36328125" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.54296875" style="2" bestFit="1" customWidth="1"/>
@@ -2026,39 +1464,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="28" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2084,10 +1522,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2113,10 +1551,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2142,10 +1580,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2171,10 +1609,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>98</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2200,10 +1638,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2229,10 +1667,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -2258,10 +1696,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -2287,31 +1725,31 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="25">
         <v>-9996</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="25">
         <v>-9996</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="25">
         <v>-9996</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="25">
         <v>-9996</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I10" s="2">
+      <c r="H10" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="25">
         <v>-9996</v>
       </c>
     </row>
@@ -2322,6 +1760,785 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C433B836-2E24-4019-9D1B-300F5E0548AB}">
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" style="1" customWidth="1"/>
+    <col min="2" max="12" width="20.54296875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="8" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="8" customFormat="1" ht="78" x14ac:dyDescent="0.35">
+      <c r="A4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33">
+        <v>-8888</v>
+      </c>
+      <c r="F7" s="33">
+        <v>-1111</v>
+      </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33">
+        <v>-9999</v>
+      </c>
+      <c r="I7" s="33">
+        <v>-9999</v>
+      </c>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33">
+        <v>-2222</v>
+      </c>
+      <c r="D9" s="33">
+        <v>-2221</v>
+      </c>
+      <c r="E9" s="33">
+        <v>-8888</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33">
+        <v>-8887</v>
+      </c>
+      <c r="H9" s="33">
+        <v>-9999</v>
+      </c>
+      <c r="I9" s="33">
+        <v>-9998</v>
+      </c>
+      <c r="J9" s="33">
+        <v>-9997</v>
+      </c>
+      <c r="K9" s="33">
+        <v>-9996</v>
+      </c>
+      <c r="L9" s="33">
+        <v>-9995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33">
+        <v>-222222222</v>
+      </c>
+      <c r="D10" s="33">
+        <v>-222222221</v>
+      </c>
+      <c r="E10" s="33">
+        <v>-888888888</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33">
+        <v>-888888887</v>
+      </c>
+      <c r="H10" s="33">
+        <v>-999999999</v>
+      </c>
+      <c r="I10" s="33">
+        <v>-999999998</v>
+      </c>
+      <c r="J10" s="33">
+        <v>-999999997</v>
+      </c>
+      <c r="K10" s="33">
+        <v>-999999996</v>
+      </c>
+      <c r="L10" s="33">
+        <v>-999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33">
+        <v>-32768</v>
+      </c>
+      <c r="D12" s="33">
+        <v>32767</v>
+      </c>
+      <c r="E12" s="33">
+        <v>-32767</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33">
+        <v>-32765</v>
+      </c>
+      <c r="H12" s="33">
+        <v>-32764</v>
+      </c>
+      <c r="I12" s="33">
+        <v>-32763</v>
+      </c>
+      <c r="J12" s="33">
+        <v>-32762</v>
+      </c>
+      <c r="K12" s="33">
+        <v>-32761</v>
+      </c>
+      <c r="L12" s="33">
+        <v>-32760</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33">
+        <v>-2147483648</v>
+      </c>
+      <c r="D13" s="33">
+        <v>2147483647</v>
+      </c>
+      <c r="E13" s="33">
+        <v>-2147483647</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33">
+        <v>-2147483645</v>
+      </c>
+      <c r="H13" s="33">
+        <v>-2147483644</v>
+      </c>
+      <c r="I13" s="33">
+        <v>-2147483643</v>
+      </c>
+      <c r="J13" s="33">
+        <v>-2147483642</v>
+      </c>
+      <c r="K13" s="33">
+        <v>-2147483641</v>
+      </c>
+      <c r="L13" s="33">
+        <v>-2147483640</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33">
+        <v>-2147483648</v>
+      </c>
+      <c r="D14" s="33">
+        <v>2147483647</v>
+      </c>
+      <c r="E14" s="33">
+        <v>-2147483647</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33">
+        <v>-2147483645</v>
+      </c>
+      <c r="H14" s="33">
+        <v>-2147483644</v>
+      </c>
+      <c r="I14" s="33">
+        <v>-2147483643</v>
+      </c>
+      <c r="J14" s="33">
+        <v>-2147483642</v>
+      </c>
+      <c r="K14" s="33">
+        <v>-2147483641</v>
+      </c>
+      <c r="L14" s="33">
+        <v>-2147483640</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="33">
+        <v>-2222</v>
+      </c>
+      <c r="D18" s="33">
+        <v>-2221</v>
+      </c>
+      <c r="E18" s="33">
+        <v>-8888</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="33">
+        <v>-8886</v>
+      </c>
+      <c r="H18" s="33">
+        <v>-9999</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="J18" s="33">
+        <v>-9997</v>
+      </c>
+      <c r="K18" s="33">
+        <v>-9996</v>
+      </c>
+      <c r="L18" s="33">
+        <v>-9995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="33">
+        <v>-2222</v>
+      </c>
+      <c r="D19" s="33">
+        <v>-2221</v>
+      </c>
+      <c r="E19" s="33">
+        <v>-8888</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G19" s="33">
+        <v>-8886</v>
+      </c>
+      <c r="H19" s="33">
+        <v>-9999</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="J19" s="33">
+        <v>-9997</v>
+      </c>
+      <c r="K19" s="33">
+        <v>-9996</v>
+      </c>
+      <c r="L19" s="33">
+        <v>-9995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="33">
+        <v>-8888</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="33">
+        <v>-8886</v>
+      </c>
+      <c r="H20" s="33">
+        <v>-9999</v>
+      </c>
+      <c r="I20" s="33">
+        <v>-9998</v>
+      </c>
+      <c r="J20" s="33">
+        <v>-9997</v>
+      </c>
+      <c r="K20" s="33">
+        <v>-9996</v>
+      </c>
+      <c r="L20" s="33">
+        <v>-9995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="33">
+        <v>-8888</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="33">
+        <v>-8886</v>
+      </c>
+      <c r="H21" s="33">
+        <v>-9999</v>
+      </c>
+      <c r="I21" s="33">
+        <v>-9998</v>
+      </c>
+      <c r="J21" s="33">
+        <v>-9997</v>
+      </c>
+      <c r="K21" s="33">
+        <v>-9996</v>
+      </c>
+      <c r="L21" s="33">
+        <v>-9995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="K22" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="L22" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="33">
+        <v>-8888</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="33">
+        <v>-8886</v>
+      </c>
+      <c r="H23" s="33">
+        <v>-9999</v>
+      </c>
+      <c r="I23" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="J23" s="33">
+        <v>-9997</v>
+      </c>
+      <c r="K23" s="33">
+        <v>-9996</v>
+      </c>
+      <c r="L23" s="33">
+        <v>-9995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="J24" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="K24" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="L24" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555A1D9B-A9E2-433A-9109-8482AB6619C1}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -2686,13 +2903,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>